<commit_message>
CAMBIOS DE SINDICATO POR SIND
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/timbrado_tmmdc_q.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/timbrado_tmmdc_q.xlsx
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="127">
   <si>
     <t>No. Empleado</t>
   </si>
@@ -521,6 +521,126 @@
   </si>
   <si>
     <t>CE CO</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
   </si>
 </sst>
 </file>
@@ -1021,22 +1141,22 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3848,10 +3968,10 @@
   <dimension ref="A1:AR141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD38"/>
+      <selection pane="bottomRight" activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,18 +4081,18 @@
       <c r="I2" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
       <c r="N2" s="63"/>
       <c r="O2" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
       <c r="T2" s="61"/>
       <c r="U2" s="62" t="s">
         <v>42</v>
@@ -3982,10 +4102,10 @@
         <v>43</v>
       </c>
       <c r="X2" s="61"/>
-      <c r="Y2" s="64" t="s">
+      <c r="Y2" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="Z2" s="65"/>
+      <c r="Z2" s="67"/>
       <c r="AA2" s="62" t="s">
         <v>44</v>
       </c>
@@ -4138,31 +4258,126 @@
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="E4" s="46"/>
-      <c r="I4" s="36"/>
-      <c r="K4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="40"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AG4" s="36"/>
-      <c r="AK4"/>
-      <c r="AL4" s="18"/>
-      <c r="AN4" s="34"/>
+      <c r="A4" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="P4" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="R4" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="S4" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="U4" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="V4" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="W4" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="X4" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y4" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z4" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA4" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB4" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC4" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD4" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE4" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF4" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG4" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH4" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI4" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ4" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK4" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL4" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM4" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN4" s="40" t="s">
+        <v>126</v>
+      </c>
       <c r="AP4" s="18"/>
       <c r="AR4" s="18"/>
     </row>
@@ -5664,11 +5879,6 @@
   </sheetData>
   <autoFilter ref="A1:AP49"/>
   <mergeCells count="15">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:T2"/>
     <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="AM2:AN2"/>
     <mergeCell ref="AG2:AH2"/>
@@ -5679,98 +5889,23 @@
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:T2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4">
+  <conditionalFormatting sqref="B4 D4 F4 H4 J4 L4 N4 P4 R4 T4 V4 X4 Z4 AB4 AD4 AF4 AH4 AJ4 AL4 AN4">
     <cfRule type="cellIs" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" priority="3" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" priority="5" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4">
-    <cfRule type="cellIs" priority="6" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" priority="7" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" priority="8" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4">
-    <cfRule type="cellIs" priority="9" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T4">
-    <cfRule type="cellIs" priority="10" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V4">
-    <cfRule type="cellIs" priority="11" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X4:Z4">
-    <cfRule type="cellIs" priority="12" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB4">
-    <cfRule type="cellIs" priority="13" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD4">
-    <cfRule type="cellIs" priority="14" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF4">
-    <cfRule type="cellIs" priority="15" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH4">
-    <cfRule type="cellIs" priority="16" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4">
-    <cfRule type="cellIs" priority="17" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL4 AL6:AL36">
+  <conditionalFormatting sqref="AL6:AL36">
     <cfRule type="cellIs" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AN4 AN6:AN36">
+  <conditionalFormatting sqref="AN6:AN36">
     <cfRule type="cellIs" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6006,34 +6141,34 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="69" t="s">
+      <c r="G2" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="J2" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="68" t="s">
+      <c r="L2" s="69" t="s">
         <v>78</v>
       </c>
       <c r="M2" s="28" t="s">
@@ -6672,16 +6807,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H2"/>
+    <mergeCell ref="I2"/>
+    <mergeCell ref="J2"/>
+    <mergeCell ref="K2"/>
+    <mergeCell ref="L2"/>
     <mergeCell ref="C2"/>
     <mergeCell ref="D2"/>
     <mergeCell ref="E2"/>
     <mergeCell ref="F2"/>
     <mergeCell ref="G2"/>
-    <mergeCell ref="H2"/>
-    <mergeCell ref="I2"/>
-    <mergeCell ref="J2"/>
-    <mergeCell ref="K2"/>
-    <mergeCell ref="L2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4">
     <cfRule type="cellIs" priority="3" operator="lessThan">

</xml_diff>